<commit_message>
Updated with next idaithalam version 1.6.2
</commit_message>
<xml_diff>
--- a/rest-db-kafka-protobuf/src/test/resources/virtualan_collection_kafka_JSON_PROTO_BUF.xlsx
+++ b/rest-db-kafka-protobuf/src/test/resources/virtualan_collection_kafka_JSON_PROTO_BUF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\microservices-lowcode-testautomation\rest-db-kafka-protobuf\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8B8025-DDE4-4FE2-8B00-035D766BC762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CC9FFF-3ED1-4FB1-9DD3-00E87B395992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -52,9 +52,6 @@
     <t>ResponseFile</t>
   </si>
   <si>
-    <t>get API testing</t>
-  </si>
-  <si>
     <t>application/json</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>GET</t>
   </si>
   <si>
-    <t>post API Testing</t>
-  </si>
-  <si>
     <t>https://live.virtualandemo.com/api/pets</t>
   </si>
   <si>
@@ -130,9 +124,6 @@
     <t>StepInfo</t>
   </si>
   <si>
-    <t>Validate pet Response</t>
-  </si>
-  <si>
     <t>contains pet information</t>
   </si>
   <si>
@@ -143,9 +134,6 @@
   </si>
   <si>
     <t>AddifyVariables</t>
-  </si>
-  <si>
-    <t>get By Id</t>
   </si>
   <si>
     <t>https://live.virtualandemo.com/api/pets/[petId]</t>
@@ -200,15 +188,6 @@
     <t>http://localhost:8800/demo/10/John</t>
   </si>
   <si>
-    <t>contains JSON  BASED information</t>
-  </si>
-  <si>
-    <t>REST_PROTO_BUF</t>
-  </si>
-  <si>
-    <t>contains PROTO BUF BASED information</t>
-  </si>
-  <si>
     <t>id,name, category/id:name,status
 i~100,doggie,i~100:string,available</t>
   </si>
@@ -230,6 +209,36 @@
   </si>
   <si>
     <t>aggregatedStdType=MSG_AGGREGATE</t>
+  </si>
+  <si>
+    <t>contains json based information</t>
+  </si>
+  <si>
+    <t>contains proto buff based information</t>
+  </si>
+  <si>
+    <t>Get by Id</t>
+  </si>
+  <si>
+    <t>Validate pet response</t>
+  </si>
+  <si>
+    <t>Get api testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post api testing with kafka aggregated </t>
+  </si>
+  <si>
+    <t>Post proto buff message</t>
+  </si>
+  <si>
+    <t>Validate Protobuff message</t>
+  </si>
+  <si>
+    <t>Kafka_aggregated</t>
+  </si>
+  <si>
+    <t>Message verification</t>
   </si>
 </sst>
 </file>
@@ -581,8 +590,8 @@
   </sheetPr>
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -590,8 +599,8 @@
     <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="61.140625" customWidth="1"/>
     <col min="7" max="7" width="24.42578125" customWidth="1"/>
     <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
@@ -609,16 +618,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>2</v>
@@ -627,13 +636,13 @@
         <v>3</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>4</v>
@@ -642,96 +651,96 @@
         <v>5</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="T1" s="10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I2" s="1">
         <v>100</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -739,17 +748,17 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="R3" s="1">
         <v>200</v>
@@ -758,39 +767,39 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="R4" s="1">
         <v>200</v>
@@ -799,37 +808,37 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -840,109 +849,109 @@
     </row>
     <row r="6" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I6" s="1">
         <v>100</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="8"/>
@@ -952,7 +961,7 @@
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
       <c r="O8" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="P8" s="7"/>
       <c r="Q8" s="8"/>
@@ -961,40 +970,40 @@
       </c>
       <c r="S8" s="8"/>
       <c r="T8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I9" s="1">
         <v>10</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="1"/>
@@ -1003,7 +1012,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with new release 1.6.3 release version
</commit_message>
<xml_diff>
--- a/rest-db-kafka-protobuf/src/test/resources/virtualan_collection_kafka_JSON_PROTO_BUF.xlsx
+++ b/rest-db-kafka-protobuf/src/test/resources/virtualan_collection_kafka_JSON_PROTO_BUF.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\microservices-lowcode-testautomation\rest-db-kafka-protobuf\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\2022\feb-release\microservices-lowcode-testautomation\rest-db-kafka-protobuf\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487B8801-FC01-49E4-A9A7-384F408E49AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57E61C9-063A-411E-9A71-F19EB38F312E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API-KAKFA-PROTOBUFF-Testing" sheetId="1" r:id="rId1"/>
@@ -235,10 +235,10 @@
     <t>Message verification</t>
   </si>
   <si>
-    <t>JSONMessageType</t>
-  </si>
-  <si>
     <t>DemoEvent</t>
+  </si>
+  <si>
+    <t>JSONType</t>
   </si>
 </sst>
 </file>
@@ -591,30 +591,30 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.27734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.27734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.140625" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.27734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.1640625" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="33" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="71.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="71.27734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="36.71875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -676,7 +676,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -695,13 +695,13 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I2" s="1">
         <v>100</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>10</v>
@@ -723,7 +723,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -766,7 +766,7 @@
       </c>
       <c r="S3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -807,7 +807,7 @@
       </c>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
@@ -848,7 +848,7 @@
       </c>
       <c r="S5" s="1"/>
     </row>
-    <row r="6" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -867,13 +867,13 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I6" s="1">
         <v>100</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
@@ -893,7 +893,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
@@ -912,11 +912,11 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -934,7 +934,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
         <v>42</v>
       </c>
@@ -974,7 +974,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>

</xml_diff>